<commit_message>
Diccionario de dato scompleto, creando entorno para inicio de sesión con mongoose, pero si no se alcanza a implementar, pensar en MySQL
</commit_message>
<xml_diff>
--- a/docs/Diccionario de Datos NoSQL- BookBox Market.xlsx
+++ b/docs/Diccionario de Datos NoSQL- BookBox Market.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Development\BookBoxMarket\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A22CB365-D0F0-4438-BFF7-2B17AEF624B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5D2A3B0-A509-485E-8589-CA9CCBCC1288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A7C4B922-BADE-4BBB-9C24-BB3CC509A90A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Diccionario Completo" sheetId="1" r:id="rId1"/>
+    <sheet name="Catálogo de Cajas Sorpresa" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="109">
   <si>
     <t>Colección</t>
   </si>
@@ -150,12 +151,6 @@
     <t>Apellido completo del usuario</t>
   </si>
   <si>
-    <t>fecha_registro</t>
-  </si>
-  <si>
-    <t>Fecha de registro del usuario</t>
-  </si>
-  <si>
     <t>Direccion de envío del usuario</t>
   </si>
   <si>
@@ -210,18 +205,12 @@
     <t>Editorial del libro.</t>
   </si>
   <si>
-    <t>Número ISBN del libro.</t>
-  </si>
-  <si>
     <t>Año de publicación del libro.</t>
   </si>
   <si>
     <t>Género literario del libro.</t>
   </si>
   <si>
-    <t>Nombre del donante (si aplica).</t>
-  </si>
-  <si>
     <t>titulo</t>
   </si>
   <si>
@@ -231,18 +220,12 @@
     <t>editorial</t>
   </si>
   <si>
-    <t>isbn</t>
-  </si>
-  <si>
     <t>anio_publicacion</t>
   </si>
   <si>
     <t>estado</t>
   </si>
   <si>
-    <t>donante</t>
-  </si>
-  <si>
     <t xml:space="preserve">Estado del libro </t>
   </si>
   <si>
@@ -288,12 +271,6 @@
     <t>Cantidad de libros incluidos en la caja.</t>
   </si>
   <si>
-    <t>Temática de la caja sorpresa.</t>
-  </si>
-  <si>
-    <t>Número único de identificación de la donación.</t>
-  </si>
-  <si>
     <t>ID del usuario que realizó la donación.</t>
   </si>
   <si>
@@ -330,9 +307,6 @@
     <t>cantidad_libros</t>
   </si>
   <si>
-    <t>tematica</t>
-  </si>
-  <si>
     <t>id_donacion</t>
   </si>
   <si>
@@ -351,9 +325,6 @@
     <t>metodo_pago</t>
   </si>
   <si>
-    <t>Número entero positivo, proviene de la colección donaciones</t>
-  </si>
-  <si>
     <t>Número entero positivo, proviene de la colección users</t>
   </si>
   <si>
@@ -367,13 +338,37 @@
   </si>
   <si>
     <t>Valor numérico, calculable</t>
+  </si>
+  <si>
+    <t>Consecutivo de la donación.</t>
+  </si>
+  <si>
+    <t>Caja Sospechosa</t>
+  </si>
+  <si>
+    <t>Caja Misteriosa</t>
+  </si>
+  <si>
+    <t>Caja Oculta</t>
+  </si>
+  <si>
+    <t>Hay un 50% de probabilidad de que los libros que aprezcan en la caja sean en base a tus preferencias</t>
+  </si>
+  <si>
+    <t>Todo será completamente aleatorio</t>
+  </si>
+  <si>
+    <t>Catálogo de Cajas Sorpresa</t>
+  </si>
+  <si>
+    <t>Hay un 80% de probabilidad de que los libros que aparezcan en la caja sean en base a tus preferencias. Por lo menos un libro será garantizado de una de tus preferencias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,8 +408,25 @@
       <color rgb="FFFFFFFF"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,6 +475,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3F3F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -491,7 +527,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -504,9 +540,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -537,6 +570,16 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,6 +588,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF3F3F"/>
       <color rgb="FFA882DA"/>
     </mruColors>
   </colors>
@@ -856,10 +900,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0EAADCE-CFF9-4829-AF0F-AD9EE6F412AD}">
-  <dimension ref="A1:E75"/>
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+      <selection activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,33 +919,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -915,721 +962,665 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="8" t="s">
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="E10" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="C12" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="E12" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="8" t="s">
+      <c r="B13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E12" s="9" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="C14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>49</v>
+      <c r="B15" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>51</v>
+        <v>18</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="9" t="s">
+      <c r="D17" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="9" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="10" t="s">
+      <c r="E18" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="E19" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="10" t="s">
+      <c r="D21" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="10" t="s">
+      <c r="C23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="10" t="s">
+      <c r="E23" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>14</v>
+        <v>65</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>70</v>
+        <v>18</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>68</v>
+        <v>65</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E26" s="9" t="s">
+      <c r="D26" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="11" t="s">
+      <c r="A27" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="9" t="s">
-        <v>8</v>
+      <c r="E27" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="9" t="s">
+      <c r="A28" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>31</v>
+      <c r="D28" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>23</v>
+      <c r="A29" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>23</v>
+      <c r="E30" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="9" t="s">
+      <c r="A31" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>110</v>
+      <c r="D31" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B32" s="10" t="s">
+      <c r="A32" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>105</v>
+      <c r="A35" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>106</v>
+        <v>68</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>107</v>
+      <c r="D37" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>27</v>
+        <v>68</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>90</v>
+        <v>68</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="E40" s="9" t="s">
-        <v>8</v>
+      <c r="A40" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>31</v>
+      <c r="A41" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>106</v>
-      </c>
+      <c r="A42" s="3"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="E43" s="9" t="s">
-        <v>108</v>
-      </c>
+      <c r="A43" s="4"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>27</v>
-      </c>
+      <c r="A44" s="4"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E45" s="9" t="s">
-        <v>109</v>
-      </c>
+      <c r="A45" s="4"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
+      <c r="A46" s="4"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
@@ -1646,35 +1637,23 @@
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
+    <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-    </row>
-    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3"/>
-    </row>
-    <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="3"/>
-    </row>
-    <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
+      <c r="A54" s="3"/>
+    </row>
+    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+    </row>
+    <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A70" s="2"/>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1683,4 +1662,60 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09A6C72-D066-43F7-8268-8C6B7916E56A}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="166.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="22"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>